<commit_message>
database and table layout
</commit_message>
<xml_diff>
--- a/info/table layout.xlsx
+++ b/info/table layout.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/APP/xampp/htdocs/roombooking/info/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
   <si>
     <t>user_id</t>
   </si>
@@ -42,9 +53,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>unique varchar 10</t>
-  </si>
-  <si>
     <t>varchar 32</t>
   </si>
   <si>
@@ -75,9 +83,6 @@
     <t>room_id</t>
   </si>
   <si>
-    <t>unique auto int</t>
-  </si>
-  <si>
     <t>room_num</t>
   </si>
   <si>
@@ -96,9 +101,6 @@
     <t>int</t>
   </si>
   <si>
-    <t>default 0, max 7 for future using</t>
-  </si>
-  <si>
     <t>building table, for future using</t>
   </si>
   <si>
@@ -108,9 +110,6 @@
     <t>default 0, 1 is not showing, for future</t>
   </si>
   <si>
-    <t>default 0, 1 is verified for future using</t>
-  </si>
-  <si>
     <t>Table attendant : tb_attendant</t>
   </si>
   <si>
@@ -183,28 +182,97 @@
     <t>datetime</t>
   </si>
   <si>
-    <t>tbl_session</t>
-  </si>
-  <si>
-    <t>ses_id</t>
-  </si>
-  <si>
-    <t>time session 30mm 1h or 2 h</t>
-  </si>
-  <si>
-    <t>default 60, can be 30, 60, 120</t>
-  </si>
-  <si>
     <t>30, 60 or 120</t>
   </si>
   <si>
     <t>tinyint</t>
+  </si>
+  <si>
+    <t>session</t>
+  </si>
+  <si>
+    <t>30, 60, 120 minutes</t>
+  </si>
+  <si>
+    <t>block_date</t>
+  </si>
+  <si>
+    <t>tb_setting</t>
+  </si>
+  <si>
+    <t>smtp</t>
+  </si>
+  <si>
+    <t>smtp server, username, password</t>
+  </si>
+  <si>
+    <t>clean_date</t>
+  </si>
+  <si>
+    <t>admin perform clean up</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>verify_code</t>
+  </si>
+  <si>
+    <t>varchr 32</t>
+  </si>
+  <si>
+    <t>login attempt, default 0, max 7 (for future using)</t>
+  </si>
+  <si>
+    <t>varchar 128</t>
+  </si>
+  <si>
+    <t>md5 ramdom for email (for future using)</t>
+  </si>
+  <si>
+    <t>default 0, 1 is verified (for future using)</t>
+  </si>
+  <si>
+    <t>admitted</t>
+  </si>
+  <si>
+    <t>notified</t>
+  </si>
+  <si>
+    <t>default 1, 1 is admitted by admin</t>
+  </si>
+  <si>
+    <t>default 0, 1 email is sent</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>1 is administrator</t>
+  </si>
+  <si>
+    <t>Database : roombooking_db</t>
+  </si>
+  <si>
+    <t>innodb, utf-8</t>
+  </si>
+  <si>
+    <t>unique varchar 11</t>
+  </si>
+  <si>
+    <t>tinyint 4</t>
+  </si>
+  <si>
+    <t>tiny text</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -222,7 +290,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -232,28 +300,42 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,337 +616,424 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H27"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36.5" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="39.7109375" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="39.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="1"/>
       <c r="F4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="1"/>
       <c r="F5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
       <c r="F6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
       <c r="F7" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D10" s="1"/>
       <c r="F10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="F13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="F14" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H14" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="C17" s="3"/>
       <c r="F17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="3" t="s">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="F20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="B25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="H26" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="F27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="F25" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>53</v>
+      <c r="H27" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>